<commit_message>
Updating rural urban Table 1
</commit_message>
<xml_diff>
--- a/output/redacted_output/hh_size_T1.xlsx
+++ b/output/redacted_output/hh_size_T1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="420">
   <si>
     <t>Table 1: Demographic and Clinical Characteristics</t>
   </si>
@@ -180,13 +180,31 @@
     <t>Yorkshire and The Humber</t>
   </si>
   <si>
-    <t>Rural-Urban</t>
-  </si>
-  <si>
-    <t>Rural</t>
-  </si>
-  <si>
-    <t>Urban</t>
+    <t>Rural-Urban Indicator</t>
+  </si>
+  <si>
+    <t>urban major conurbation</t>
+  </si>
+  <si>
+    <t>urban minor conurbation</t>
+  </si>
+  <si>
+    <t>urban city and town</t>
+  </si>
+  <si>
+    <t>urban city and town in a sparse setting</t>
+  </si>
+  <si>
+    <t>rural town and fringe</t>
+  </si>
+  <si>
+    <t>rural town and fringe in a sparse setting</t>
+  </si>
+  <si>
+    <t>rural village and dispersed</t>
+  </si>
+  <si>
+    <t>rural village and dispersed in a sparse setting</t>
   </si>
   <si>
     <t>Chronic Respiratory Diseases</t>
@@ -216,12 +234,6 @@
     <t>grouped stroke, dementia, other neurological diseases</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>grouped immunosupression or autoimmune diseases</t>
   </si>
   <si>
@@ -363,10 +375,28 @@
     <t>2146946 (14.0)</t>
   </si>
   <si>
-    <t>3119801 (20.4)</t>
-  </si>
-  <si>
-    <t>12173802 (79.6)</t>
+    <t>3121887 (20.4)</t>
+  </si>
+  <si>
+    <t>963974 (6.3)</t>
+  </si>
+  <si>
+    <t>7921368 (51.8)</t>
+  </si>
+  <si>
+    <t>23549 (0.2)</t>
+  </si>
+  <si>
+    <t>1710744 (11.2)</t>
+  </si>
+  <si>
+    <t>69362 (0.5)</t>
+  </si>
+  <si>
+    <t>1248169 (8.2)</t>
+  </si>
+  <si>
+    <t>91526 (0.6)</t>
   </si>
   <si>
     <t>14875548 (97.3)</t>
@@ -387,10 +417,10 @@
     <t>2261143 (14.8)</t>
   </si>
   <si>
-    <t>1076726 (7.0)</t>
-  </si>
-  <si>
-    <t>14216877 (93.0)</t>
+    <t>15293603 (100.0)</t>
+  </si>
+  <si>
+    <t>0 (0.0)</t>
   </si>
   <si>
     <t>15231549 (99.6)</t>
@@ -555,10 +585,28 @@
     <t>1157031 (13.8)</t>
   </si>
   <si>
-    <t>1928957 (23.0)</t>
-  </si>
-  <si>
-    <t>6471455 (77.0)</t>
+    <t>1472866 (17.5)</t>
+  </si>
+  <si>
+    <t>542167 (6.5)</t>
+  </si>
+  <si>
+    <t>4356135 (51.9)</t>
+  </si>
+  <si>
+    <t>15282 (0.2)</t>
+  </si>
+  <si>
+    <t>1038079 (12.4)</t>
+  </si>
+  <si>
+    <t>45307 (0.5)</t>
+  </si>
+  <si>
+    <t>783457 (9.3)</t>
+  </si>
+  <si>
+    <t>62114 (0.7)</t>
   </si>
   <si>
     <t>8056736 (95.9)</t>
@@ -579,10 +627,7 @@
     <t>1809676 (21.5)</t>
   </si>
   <si>
-    <t>778212 (9.3)</t>
-  </si>
-  <si>
-    <t>7622200 (90.7)</t>
+    <t>8400412 (100.0)</t>
   </si>
   <si>
     <t>8355689 (99.5)</t>
@@ -747,10 +792,28 @@
     <t>735184 (13.9)</t>
   </si>
   <si>
-    <t>1013820 (19.2)</t>
-  </si>
-  <si>
-    <t>4265020 (80.8)</t>
+    <t>1112121 (21.1)</t>
+  </si>
+  <si>
+    <t>329770 (6.2)</t>
+  </si>
+  <si>
+    <t>2765120 (52.4)</t>
+  </si>
+  <si>
+    <t>6538 (0.1)</t>
+  </si>
+  <si>
+    <t>574517 (10.9)</t>
+  </si>
+  <si>
+    <t>20082 (0.4)</t>
+  </si>
+  <si>
+    <t>394928 (7.5)</t>
+  </si>
+  <si>
+    <t>24293 (0.5)</t>
   </si>
   <si>
     <t>5221473 (98.9)</t>
@@ -771,10 +834,7 @@
     <t>346503 (6.6)</t>
   </si>
   <si>
-    <t>211169 (4.0)</t>
-  </si>
-  <si>
-    <t>5067671 (96.0)</t>
+    <t>5278840 (100.0)</t>
   </si>
   <si>
     <t>5266287 (99.8)</t>
@@ -939,10 +999,28 @@
     <t>188861 (15.6)</t>
   </si>
   <si>
-    <t>146784 (12.2)</t>
-  </si>
-  <si>
-    <t>1060269 (87.8)</t>
+    <t>372490 (30.9)</t>
+  </si>
+  <si>
+    <t>70538 (5.8)</t>
+  </si>
+  <si>
+    <t>610225 (50.6)</t>
+  </si>
+  <si>
+    <t>1443 (0.1)</t>
+  </si>
+  <si>
+    <t>82267 (6.8)</t>
+  </si>
+  <si>
+    <t>3307 (0.3)</t>
+  </si>
+  <si>
+    <t>57029 (4.7)</t>
+  </si>
+  <si>
+    <t>4181 (0.3)</t>
   </si>
   <si>
     <t>1193997 (98.9)</t>
@@ -963,10 +1041,7 @@
     <t>78218 (6.5)</t>
   </si>
   <si>
-    <t>62443 (5.2)</t>
-  </si>
-  <si>
-    <t>1144610 (94.8)</t>
+    <t>1207053 (100.0)</t>
   </si>
   <si>
     <t>1203628 (99.7)</t>
@@ -1131,10 +1206,28 @@
     <t>65870 (16.2)</t>
   </si>
   <si>
-    <t>30240 (7.4)</t>
-  </si>
-  <si>
-    <t>377058 (92.6)</t>
+    <t>164410 (40.4)</t>
+  </si>
+  <si>
+    <t>21499 (5.3)</t>
+  </si>
+  <si>
+    <t>189888 (46.6)</t>
+  </si>
+  <si>
+    <t>286 (0.1)</t>
+  </si>
+  <si>
+    <t>15881 (3.9)</t>
+  </si>
+  <si>
+    <t>666 (0.2)</t>
+  </si>
+  <si>
+    <t>12755 (3.1)</t>
+  </si>
+  <si>
+    <t>938 (0.2)</t>
   </si>
   <si>
     <t>403342 (99.0)</t>
@@ -1155,10 +1248,7 @@
     <t>26746 (6.6)</t>
   </si>
   <si>
-    <t>24902 (6.1)</t>
-  </si>
-  <si>
-    <t>382396 (93.9)</t>
+    <t>407298 (100.0)</t>
   </si>
   <si>
     <t>405945 (99.7)</t>
@@ -1228,7 +1318,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G88"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1257,19 +1347,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="F2" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1299,19 +1389,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="F4" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1320,19 +1410,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="E5" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="F5" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1362,19 +1452,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="E7" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="F7" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1383,19 +1473,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="E8" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="F8" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -1425,19 +1515,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="E10" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="F10" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1446,19 +1536,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D11" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="E11" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="F11" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1467,19 +1557,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E12" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="F12" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1488,19 +1578,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="E13" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="F13" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1509,19 +1599,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D14" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E14" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="F14" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1530,19 +1620,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="E15" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="F15" t="s">
-        <v>336</v>
+        <v>361</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1551,19 +1641,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D16" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="E16" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="F16" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1572,19 +1662,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="E17" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="F17" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -1593,19 +1683,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="D18" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="E18" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="F18" t="s">
-        <v>339</v>
+        <v>364</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -1614,19 +1704,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="D19" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="E19" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="F19" t="s">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -1635,19 +1725,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D20" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="E20" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="F20" t="s">
-        <v>341</v>
+        <v>366</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1656,19 +1746,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D21" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="E21" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="F21" t="s">
-        <v>342</v>
+        <v>367</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1698,19 +1788,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D23" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="E23" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="F23" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1719,19 +1809,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D24" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="E24" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="F24" t="s">
-        <v>344</v>
+        <v>369</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1740,19 +1830,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D25" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="E25" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="F25" t="s">
-        <v>345</v>
+        <v>370</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1761,19 +1851,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="E26" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="F26" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -1782,19 +1872,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D27" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="E27" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="F27" t="s">
-        <v>347</v>
+        <v>372</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -1824,19 +1914,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="D29" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E29" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="F29" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1845,19 +1935,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D30" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="E30" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="F30" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1866,19 +1956,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D31" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="E31" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="F31" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1887,19 +1977,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D32" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="E32" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
       <c r="F32" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -1908,19 +1998,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D33" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="E33" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="F33" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1929,19 +2019,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D34" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="E34" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F34" t="s">
-        <v>353</v>
+        <v>378</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1971,19 +2061,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="E36" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="F36" t="s">
-        <v>354</v>
+        <v>379</v>
       </c>
       <c r="G36" s="1"/>
     </row>
@@ -1992,19 +2082,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D37" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="E37" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="F37" t="s">
-        <v>355</v>
+        <v>380</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -2013,19 +2103,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="D38" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="E38" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="F38" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -2034,19 +2124,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="E39" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="F39" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -2076,19 +2166,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D41" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="E41" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="F41" t="s">
-        <v>358</v>
+        <v>383</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -2097,19 +2187,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D42" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="E42" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="F42" t="s">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -2118,19 +2208,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D43" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="E43" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="F43" t="s">
-        <v>360</v>
+        <v>385</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -2139,19 +2229,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D44" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="E44" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="F44" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -2160,19 +2250,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D45" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="E45" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="F45" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -2202,19 +2292,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D47" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="E47" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="F47" t="s">
-        <v>363</v>
+        <v>388</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -2223,19 +2313,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D48" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="E48" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="F48" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -2244,19 +2334,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D49" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="E49" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="F49" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -2265,19 +2355,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D50" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E50" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="F50" t="s">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -2286,19 +2376,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C51" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D51" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="E51" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="F51" t="s">
-        <v>367</v>
+        <v>392</v>
       </c>
       <c r="G51" s="1"/>
     </row>
@@ -2307,19 +2397,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D52" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="E52" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="F52" t="s">
-        <v>368</v>
+        <v>393</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -2328,19 +2418,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="D53" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="E53" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="F53" t="s">
-        <v>369</v>
+        <v>394</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -2349,19 +2439,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D54" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="E54" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="F54" t="s">
-        <v>370</v>
+        <v>395</v>
       </c>
       <c r="G54" s="1"/>
     </row>
@@ -2370,19 +2460,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D55" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="E55" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="F55" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
       <c r="G55" s="1"/>
     </row>
@@ -2412,19 +2502,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="D57" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="E57" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="F57" t="s">
-        <v>372</v>
+        <v>397</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -2433,19 +2523,19 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="D58" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="E58" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="F58" t="s">
-        <v>373</v>
+        <v>398</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2454,19 +2544,19 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>1</v>
+        <v>192</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>261</v>
       </c>
       <c r="E59" t="s">
-        <v>1</v>
+        <v>330</v>
       </c>
       <c r="F59" t="s">
-        <v>1</v>
+        <v>399</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2475,19 +2565,19 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="D60" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="E60" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="F60" t="s">
-        <v>374</v>
+        <v>400</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2496,19 +2586,19 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C61" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="D61" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="E61" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="F61" t="s">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -2517,67 +2607,67 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="D62" t="s">
-        <v>1</v>
+        <v>264</v>
       </c>
       <c r="E62" t="s">
-        <v>1</v>
+        <v>333</v>
       </c>
       <c r="F62" t="s">
-        <v>1</v>
+        <v>402</v>
       </c>
       <c r="G62" s="1"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="D63" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="E63" t="s">
-        <v>312</v>
+        <v>334</v>
       </c>
       <c r="F63" t="s">
-        <v>376</v>
+        <v>403</v>
       </c>
       <c r="G63" s="1"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D64" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="E64" t="s">
-        <v>313</v>
+        <v>335</v>
       </c>
       <c r="F64" t="s">
-        <v>377</v>
+        <v>404</v>
       </c>
       <c r="G64" s="1"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
@@ -2598,49 +2688,49 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C66" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="D66" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="E66" t="s">
-        <v>314</v>
+        <v>336</v>
       </c>
       <c r="F66" t="s">
-        <v>378</v>
+        <v>405</v>
       </c>
       <c r="G66" s="1"/>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C67" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="D67" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="E67" t="s">
-        <v>315</v>
+        <v>337</v>
       </c>
       <c r="F67" t="s">
-        <v>379</v>
+        <v>406</v>
       </c>
       <c r="G67" s="1"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
@@ -2661,49 +2751,49 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="D69" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="E69" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
       <c r="F69" t="s">
-        <v>380</v>
+        <v>407</v>
       </c>
       <c r="G69" s="1"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="D70" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="E70" t="s">
-        <v>317</v>
+        <v>339</v>
       </c>
       <c r="F70" t="s">
-        <v>381</v>
+        <v>408</v>
       </c>
       <c r="G70" s="1"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
@@ -2724,49 +2814,49 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C72" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="D72" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="E72" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
       <c r="F72" t="s">
-        <v>382</v>
+        <v>409</v>
       </c>
       <c r="G72" s="1"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C73" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="D73" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="E73" t="s">
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="F73" t="s">
-        <v>383</v>
+        <v>410</v>
       </c>
       <c r="G73" s="1"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -2787,49 +2877,49 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C75" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="D75" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="E75" t="s">
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="F75" t="s">
-        <v>384</v>
+        <v>411</v>
       </c>
       <c r="G75" s="1"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C76" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="D76" t="s">
-        <v>257</v>
+        <v>135</v>
       </c>
       <c r="E76" t="s">
-        <v>321</v>
+        <v>135</v>
       </c>
       <c r="F76" t="s">
-        <v>385</v>
+        <v>135</v>
       </c>
       <c r="G76" s="1"/>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
@@ -2850,49 +2940,49 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C78" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="D78" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="E78" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="F78" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="G78" s="1"/>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="D79" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="E79" t="s">
-        <v>323</v>
+        <v>344</v>
       </c>
       <c r="F79" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
@@ -2913,45 +3003,171 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B81" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C81" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="D81" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="E81" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
       <c r="F81" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="G81" s="1"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B82" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C82" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="D82" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="E82" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
       <c r="F82" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="G82" s="1"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>72</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>65</v>
+      </c>
+      <c r="B84" t="s">
+        <v>140</v>
+      </c>
+      <c r="C84" t="s">
+        <v>209</v>
+      </c>
+      <c r="D84" t="s">
+        <v>278</v>
+      </c>
+      <c r="E84" t="s">
+        <v>347</v>
+      </c>
+      <c r="F84" t="s">
+        <v>416</v>
+      </c>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>66</v>
+      </c>
+      <c r="B85" t="s">
+        <v>141</v>
+      </c>
+      <c r="C85" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" t="s">
+        <v>279</v>
+      </c>
+      <c r="E85" t="s">
+        <v>348</v>
+      </c>
+      <c r="F85" t="s">
+        <v>417</v>
+      </c>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>73</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>65</v>
+      </c>
+      <c r="B87" t="s">
+        <v>142</v>
+      </c>
+      <c r="C87" t="s">
+        <v>211</v>
+      </c>
+      <c r="D87" t="s">
+        <v>280</v>
+      </c>
+      <c r="E87" t="s">
+        <v>349</v>
+      </c>
+      <c r="F87" t="s">
+        <v>418</v>
+      </c>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>66</v>
+      </c>
+      <c r="B88" t="s">
+        <v>143</v>
+      </c>
+      <c r="C88" t="s">
+        <v>212</v>
+      </c>
+      <c r="D88" t="s">
+        <v>281</v>
+      </c>
+      <c r="E88" t="s">
+        <v>350</v>
+      </c>
+      <c r="F88" t="s">
+        <v>419</v>
+      </c>
+      <c r="G88" s="1"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>